<commit_message>
Revert "Merge branch 'master' of https://github.com/COISPA/RoME"
This reverts commit e7f21df63eefa4b5d96a9fdc0c19bea89d90c431, reversing
changes made to 0e943d0555bf277b14a2a2cb866462194225a3c9.
</commit_message>
<xml_diff>
--- a/lista_file.xlsx
+++ b/lista_file.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents and Settings\Utente\Documenti\GitHub\RoME\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
   </bookViews>
@@ -19,7 +24,7 @@
     <author>Walter</author>
   </authors>
   <commentList>
-    <comment ref="A2" authorId="0">
+    <comment ref="A2" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -48,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="68">
   <si>
     <t>check_0_fieldsTA.r</t>
   </si>
@@ -1063,7 +1068,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1073,8 +1078,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D64"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1572,9 +1577,6 @@
       <c r="B47" t="s">
         <v>32</v>
       </c>
-      <c r="C47" t="s">
-        <v>2</v>
-      </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">

</xml_diff>